<commit_message>
with vid behavior offset
</commit_message>
<xml_diff>
--- a/Animal_ID_Info.xlsx
+++ b/Animal_ID_Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd Appleby\Documents\SCIENCE\Fent\SAPaper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF4F560D-F05E-4DD0-A603-442FBA8B653D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863CFC4F-95AF-4334-BBB1-23F91BA1EF6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{681EA8E8-EE67-4E68-ABCC-088CB50E542B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>VIDEO</t>
   </si>
@@ -90,13 +90,16 @@
   </si>
   <si>
     <t>R2024-09-17_13-00-32_BOX4_PM</t>
+  </si>
+  <si>
+    <t>Operant Start (seconds)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +119,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -175,6 +186,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{138CE161-C763-470D-8C0A-870D3FF9D325}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +533,7 @@
     <col min="1" max="1" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,8 +549,11 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -553,8 +569,11 @@
       <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -570,8 +589,11 @@
       <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="8">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -587,8 +609,11 @@
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="8">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -604,8 +629,11 @@
       <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="8">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -621,8 +649,11 @@
       <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -638,8 +669,11 @@
       <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -655,8 +689,11 @@
       <c r="E8" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -672,8 +709,11 @@
       <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="8">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -689,8 +729,11 @@
       <c r="E10" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="8">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -706,8 +749,11 @@
       <c r="E11" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="8">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
@@ -723,22 +769,25 @@
       <c r="E12" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="8">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>

</xml_diff>